<commit_message>
Refactor String to color conversion & definition of rgb colors
</commit_message>
<xml_diff>
--- a/Ressources/Todo.xlsx
+++ b/Ressources/Todo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas\Documents\Github\Alpha\Ressources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -444,7 +444,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -496,7 +496,7 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F3" t="s">
         <v>5</v>
@@ -538,7 +538,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Full scrollbar  support in console
</commit_message>
<xml_diff>
--- a/Ressources/Todo.xlsx
+++ b/Ressources/Todo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="21">
   <si>
     <t>Add padding to text</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>Render base terrain</t>
+  </si>
+  <si>
+    <t>Implement scrolling with mouse</t>
   </si>
 </sst>
 </file>
@@ -444,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,7 +533,7 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -574,7 +577,7 @@
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -597,6 +600,17 @@
       </c>
       <c r="C11" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Successful iterative delaunay triangulation used for map generation
</commit_message>
<xml_diff>
--- a/Ressources/Todo.xlsx
+++ b/Ressources/Todo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="23">
   <si>
     <t>Add padding to text</t>
   </si>
@@ -87,6 +87,12 @@
   </si>
   <si>
     <t>Implement scrolling with mouse</t>
+  </si>
+  <si>
+    <t>Incremental zoom on scrool</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -447,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -611,6 +617,22 @@
       </c>
       <c r="C12" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>